<commit_message>
arreglado versión php para que funcione en el hosting
</commit_message>
<xml_diff>
--- a/InscripcionesEVG/controllers/torneo.xlsx
+++ b/InscripcionesEVG/controllers/torneo.xlsx
@@ -492,6 +492,15 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
@@ -577,5 +586,14 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ya genera excel para cada prueba
</commit_message>
<xml_diff>
--- a/InscripcionesEVG/controllers/torneo.xlsx
+++ b/InscripcionesEVG/controllers/torneo.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Ciclos - F - 800 metros" sheetId="1" r:id="rId4"/>
-    <sheet name="Ciclos - M - 800 metros" sheetId="2" r:id="rId5"/>
+    <sheet name="Ciclos - F - 4_100 metros" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -16,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>INSCRIPCIONES TORNEO OLÍMPICO</t>
   </si>
   <si>
-    <t>800 metros    FEMENINA</t>
+    <t>4*100 metros    FEMENINA</t>
   </si>
   <si>
     <t>Ciclos</t>
@@ -42,22 +41,10 @@
     <t>Laura, Gómez</t>
   </si>
   <si>
-    <t>800 metros    MASCULINA</t>
-  </si>
-  <si>
-    <t>Javier, Torres</t>
-  </si>
-  <si>
-    <t>José, Ruiz</t>
-  </si>
-  <si>
-    <t>2DAW</t>
-  </si>
-  <si>
-    <t>Pedro, Sánchez</t>
-  </si>
-  <si>
-    <t>Sergio, Molina</t>
+    <t>María, López</t>
+  </si>
+  <si>
+    <t>Paula, Díaz</t>
   </si>
 </sst>
 </file>
@@ -431,84 +418,6 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A6" sqref="A6:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="true" style="0"/>
-    <col min="2" max="2" width="15" customWidth="true" style="0"/>
-    <col min="3" max="3" width="15" customWidth="true" style="0"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" customHeight="1" ht="30">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
@@ -529,7 +438,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -547,7 +456,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -555,15 +464,15 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -571,10 +480,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>